<commit_message>
Added results for fallacy fallacy
</commit_message>
<xml_diff>
--- a/Results/tanksoar_self_motivated.xlsx
+++ b/Results/tanksoar_self_motivated.xlsx
@@ -14,10 +14,7 @@
   <sheets>
     <sheet name="tanksoar_self_motivated" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2889,103 +2886,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="tanksoar_self_motivated"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="N4" t="str">
-            <v>Missiles Fired</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="N5" t="str">
-            <v>Tank 1</v>
-          </cell>
-          <cell r="O5" t="str">
-            <v>Tank 2</v>
-          </cell>
-          <cell r="P5" t="str">
-            <v>Tank 3</v>
-          </cell>
-          <cell r="Q5" t="str">
-            <v>Tank 4</v>
-          </cell>
-          <cell r="T5" t="str">
-            <v>Tank 1</v>
-          </cell>
-          <cell r="U5" t="str">
-            <v>Tank 2</v>
-          </cell>
-          <cell r="V5" t="str">
-            <v>Tank 3</v>
-          </cell>
-          <cell r="W5" t="str">
-            <v>Tank 4</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="N10">
-            <v>0.12015139606131836</v>
-          </cell>
-          <cell r="O10">
-            <v>0.67846501752835775</v>
-          </cell>
-          <cell r="P10">
-            <v>0.12809500159630263</v>
-          </cell>
-          <cell r="Q10">
-            <v>0.68319362827594421</v>
-          </cell>
-          <cell r="T10">
-            <v>0.10547699671000343</v>
-          </cell>
-          <cell r="U10">
-            <v>7.4190870215937954E-2</v>
-          </cell>
-          <cell r="V10">
-            <v>0.10071062371466712</v>
-          </cell>
-          <cell r="W10">
-            <v>7.5171213783918223E-2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="N13">
-            <v>1.3029999999999999</v>
-          </cell>
-          <cell r="O13">
-            <v>32.04</v>
-          </cell>
-          <cell r="P13">
-            <v>1.385</v>
-          </cell>
-          <cell r="Q13">
-            <v>31.952999999999999</v>
-          </cell>
-          <cell r="T13">
-            <v>3.9580000000000002</v>
-          </cell>
-          <cell r="U13">
-            <v>1.506</v>
-          </cell>
-          <cell r="V13">
-            <v>3.8109999999999999</v>
-          </cell>
-          <cell r="W13">
-            <v>1.4930000000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3252,7 +3152,7 @@
   <dimension ref="A1:W401"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3732,7 +3632,7 @@
         <v>100</v>
       </c>
       <c r="Q9" s="1">
-        <f t="array" ref="Q9">COUNT(IF(MOD(ROW($E$2:$E$4001)-2,4)=3,$E$2:$E$401))</f>
+        <f t="array" ref="Q9">COUNT(IF(MOD(ROW($E$2:$E$401)-2,4)=3,$E$2:$E$401))</f>
         <v>100</v>
       </c>
       <c r="R9" s="1"/>

</xml_diff>